<commit_message>
Week 5 - Update...
</commit_message>
<xml_diff>
--- a/Workbook1 (Autosaved) (Autosaved).xlsx
+++ b/Workbook1 (Autosaved) (Autosaved).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2356,15 +2356,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>412658</xdr:colOff>
+      <xdr:colOff>565058</xdr:colOff>
       <xdr:row>56</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>30</xdr:col>
-      <xdr:colOff>594137</xdr:colOff>
+      <xdr:colOff>746537</xdr:colOff>
       <xdr:row>71</xdr:row>
-      <xdr:rowOff>56948</xdr:rowOff>
+      <xdr:rowOff>69648</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2387,7 +2387,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="23526658" y="11423650"/>
+          <a:off x="23679058" y="11436350"/>
           <a:ext cx="1832479" cy="3060498"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2400,15 +2400,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>373380</xdr:colOff>
+      <xdr:colOff>449580</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>103156</xdr:rowOff>
+      <xdr:rowOff>115856</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>147320</xdr:colOff>
+      <xdr:colOff>223520</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>114051</xdr:rowOff>
+      <xdr:rowOff>126751</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2431,7 +2431,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="24312880" y="10872756"/>
+          <a:off x="24389080" y="10885456"/>
           <a:ext cx="1424940" cy="1026895"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2444,15 +2444,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>30</xdr:col>
-      <xdr:colOff>83290</xdr:colOff>
+      <xdr:colOff>157703</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>120650</xdr:rowOff>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>30</xdr:col>
-      <xdr:colOff>547027</xdr:colOff>
+      <xdr:colOff>621440</xdr:colOff>
       <xdr:row>56</xdr:row>
-      <xdr:rowOff>185704</xdr:rowOff>
+      <xdr:rowOff>198404</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2475,7 +2475,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="24848290" y="11093450"/>
+          <a:off x="24922703" y="11106150"/>
           <a:ext cx="463737" cy="471454"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2565,6 +2565,94 @@
         <a:xfrm>
           <a:off x="30689341" y="12365054"/>
           <a:ext cx="2902857" cy="3097143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>43</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>94594</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>72551</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId49">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="35778966" y="12466437"/>
+          <a:ext cx="2590800" cy="2933700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId50">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="31369000" y="17881600"/>
+          <a:ext cx="2908300" cy="3073400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2841,8 +2929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="G6:M43"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="AA40" workbookViewId="0">
-      <selection activeCell="AP72" sqref="AP72"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="Y40" workbookViewId="0">
+      <selection activeCell="AJ98" sqref="AJ98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>